<commit_message>
New Changes have been made!!
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/HRMLogin.xlsx
+++ b/src/test/resources/testdata/HRMLogin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faris\eclipse-workspace\HybridFrameworkOrangeHRM\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FFF60F6-1D4D-4A15-93DA-F8B5C42EB482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6540102C-D852-48A4-983B-DC04594ECC2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>Faris198407</t>
-  </si>
-  <si>
     <t>Admin1</t>
   </si>
   <si>
@@ -63,6 +60,9 @@
   </si>
   <si>
     <t>Ward</t>
+  </si>
+  <si>
+    <t>admin123</t>
   </si>
 </sst>
 </file>
@@ -433,8 +433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -456,7 +456,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -488,10 +488,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -506,7 +506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B8D684-1AB9-4753-9C59-92A4BE4B38BF}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -530,24 +530,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Test Scripts with the updated URL!!
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/HRMLogin.xlsx
+++ b/src/test/resources/testdata/HRMLogin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faris\eclipse-workspace\HybridFrameworkOrangeHRM\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6540102C-D852-48A4-983B-DC04594ECC2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C371DB-EF97-439B-A129-067E5CA3C351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
     <t>Ward</t>
   </si>
   <si>
-    <t>admin123</t>
+    <t>Faris198407</t>
   </si>
 </sst>
 </file>
@@ -434,7 +434,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>